<commit_message>
Further cleanup on TNP Reporting Manual.xlsx.
</commit_message>
<xml_diff>
--- a/TNP Reporting Manual.xlsx
+++ b/TNP Reporting Manual.xlsx
@@ -20,9 +20,9 @@
   </sheets>
   <calcPr calcId="140000"/>
   <customWorkbookViews>
+    <customWorkbookView name="MONIQUE - Personal View" guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="785" tabRatio="500" activeSheetId="2"/>
+    <customWorkbookView name="Unisys - Personal View" guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jonathan Levy - Personal View" guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1066" tabRatio="500" activeSheetId="5"/>
-    <customWorkbookView name="Unisys - Personal View" guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="MONIQUE - Personal View" guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="785" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>The date and time of when the trip ended. All times must be either local or the time zone must be noted per ISO 8601 specifications.</t>
-  </si>
-  <si>
-    <t>The Census Block 2010 corresponding to the starting location of the trip.</t>
   </si>
   <si>
     <t>The Census Block 2010 corresponding to the ending location of the trip.</t>
@@ -483,12 +480,29 @@
       <t xml:space="preserve"> by the file (not the period when the file is submitted). For instance, ACME service submitting the driver file of drivers eligible in March 2016 would submit acme-driver-201603.csv.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Census Block 2010 corresponding to the starting location of the trip.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -522,6 +536,14 @@
     </font>
     <font>
       <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -676,7 +698,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FDBC06D3-9E0D-4DCA-9B0A-EAB13DF0C855}" diskRevisions="1" revisionId="87" version="9">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DA3DC931-C2F3-483F-A5F5-1B1BEE67700A}" diskRevisions="1" revisionId="89" version="11">
   <header guid="{88FB6579-DFE5-4318-B552-D049D04FAB73}" dateTime="2016-10-13T12:50:22" maxSheetId="5" userName="Jonathan Levy" r:id="rId16" minRId="76">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -734,6 +756,24 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{9DFAB7F4-9EC9-4A0F-ACF7-77494652790A}" dateTime="2016-10-14T11:37:08" maxSheetId="6" userName="Jonathan Levy" r:id="rId23" minRId="88">
+    <sheetIdMap count="5">
+      <sheetId val="5"/>
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DA3DC931-C2F3-483F-A5F5-1B1BEE67700A}" dateTime="2016-10-14T11:37:36" maxSheetId="6" userName="Jonathan Levy" r:id="rId24" minRId="89">
+    <sheetIdMap count="5">
+      <sheetId val="5"/>
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -930,6 +970,80 @@
   </rcc>
   <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
   <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcmt sheetId="3" cell="E7" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Jonathan Levy"/>
+  <rcc rId="88" sId="3">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <t>The Census Block 2010 corresponding to the starting location of the trip.</t>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">The Census Block 2010 corresponding to the starting location of the trip.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.  TNPs interested in doing so should discuss it with the City of Chicago.)</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="89" sId="3">
+    <oc r="E7" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">The Census Block 2010 corresponding to the starting location of the trip.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.  TNPs interested in doing so should discuss it with the City of Chicago.)</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E7" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">The Census Block 2010 corresponding to the starting location of the trip.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.)</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -1261,9 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1272,12 +1384,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1422,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1490,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1417,520 +1529,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="A3" sqref="A3"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" scale="125" showPageBreaks="1">
+      <selection activeCell="D11" sqref="D11"/>
+      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
     <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" scale="125">
       <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" scale="125" showPageBreaks="1">
-      <selection activeCell="D11" sqref="D11"/>
-      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
-    </customSheetView>
-  </customSheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <customSheetViews>
     <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="B10" sqref="B10"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
-      <selection activeCell="C8" sqref="C8"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" showPageBreaks="1">
-      <selection activeCell="E7" sqref="E7"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-    </customSheetView>
-  </customSheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <customSheetViews>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="E11" sqref="E11"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" topLeftCell="A10">
+      <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -1945,12 +1555,514 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" showPageBreaks="1">
+      <selection activeCell="E7" sqref="E7"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
+      <selection activeCell="C8" sqref="C8"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+      <selection activeCell="B10" sqref="B10"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" topLeftCell="A10">
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+      <selection activeCell="E11" sqref="E11"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1963,7 +2075,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,7 +2143,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -2053,7 +2165,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}">
       <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2063,7 +2175,7 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}">
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
       <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2080,12 +2192,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2235,15 +2344,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2267,17 +2387,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edited TNP Reporting Manual.xlsx / Trip to clarify the definition of a trip in the context of trip sharing.
</commit_message>
<xml_diff>
--- a/TNP Reporting Manual.xlsx
+++ b/TNP Reporting Manual.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Analytics\TNP\tnp-reporting-manual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Analytics\TNP\Related_Projects\tnp-reporting-manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="22620" windowHeight="13170" tabRatio="500"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="22620" windowHeight="13170" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="File Names" sheetId="5" r:id="rId1"/>
@@ -20,9 +20,9 @@
   </sheets>
   <calcPr calcId="140000"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jonathan Levy - Personal View" guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1066" tabRatio="500" activeSheetId="3"/>
+    <customWorkbookView name="Unisys - Personal View" guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="MONIQUE - Personal View" guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="785" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Unisys - Personal View" guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jonathan Levy - Personal View" guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1066" tabRatio="500" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -283,50 +283,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>All vehicles eligible at any point during the reporting period.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Scope: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">All Trips </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>completed</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> during the reporting period.  Trips in progress at the end of the reporting period should be held for the next report.</t>
     </r>
   </si>
   <si>
@@ -495,6 +451,50 @@
         <scheme val="minor"/>
       </rPr>
       <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scope: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">All Trips </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>completed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> during the reporting period.  Trips in progress at the end of the reporting period should be held for the next report.  For the purposes of this file, a trip is a transaction with a specific customer, including any additional people transported under the same transaction. A transaction with a different customer, even if present in the vehicle at the same time, is a separate trip.</t>
     </r>
   </si>
 </sst>
@@ -615,7 +615,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -636,6 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -698,7 +699,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DA3DC931-C2F3-483F-A5F5-1B1BEE67700A}" diskRevisions="1" revisionId="89" version="11">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{71B4191B-0BAA-4279-8855-B887A7C7CB4D}" diskRevisions="1" revisionId="90" version="12">
   <header guid="{88FB6579-DFE5-4318-B552-D049D04FAB73}" dateTime="2016-10-13T12:50:22" maxSheetId="5" userName="Jonathan Levy" r:id="rId16" minRId="76">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -774,6 +775,15 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{71B4191B-0BAA-4279-8855-B887A7C7CB4D}" dateTime="2017-05-15T15:44:47" maxSheetId="6" userName="Jonathan Levy" r:id="rId25" minRId="90">
+    <sheetIdMap count="5">
+      <sheetId val="5"/>
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -791,6 +801,149 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="3" sqref="A1" start="0" length="0">
+    <dxf>
+      <alignment vertical="top" wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1">
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1">
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1" start="0" length="0">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1">
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1" start="0" length="0">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1">
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1" start="0" length="0">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="A1:E1">
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="90" sId="3">
+    <oc r="A1" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Scope: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">All Trips </t>
+        </r>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>completed</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> during the reporting period.  Trips in progress at the end of the reporting period should be held for the next report.</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="A1" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Scope: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">All Trips </t>
+        </r>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>completed</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> during the reporting period.  Trips in progress at the end of the reporting period should be held for the next report.  For the purposes of this file, a trip is a transaction with a specific customer, including any additional people transported under the same transaction. A transaction with a different customer, even if present in the vehicle at the same time, is a separate trip.</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
+  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="add"/>
 </revisions>
 </file>
 
@@ -1048,7 +1201,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{71B4191B-0BAA-4279-8855-B887A7C7CB4D}" name="Jonathan Levy" id="-1743086255" dateTime="2017-05-15T14:18:15"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1375,7 +1530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1384,12 +1541,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1647,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,20 +1686,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" scale="125" showPageBreaks="1">
-      <selection activeCell="D11" sqref="D11"/>
-      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+      <selection activeCell="A3" sqref="A3"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" scale="125">
       <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="A3" sqref="A3"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" scale="125" showPageBreaks="1">
+      <selection activeCell="D11" sqref="D11"/>
+      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1560,7 +1717,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1763,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1640,7 +1797,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,7 +1848,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,7 +1865,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
@@ -1725,7 +1882,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
@@ -1742,25 +1899,25 @@
         <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" showPageBreaks="1">
-      <selection activeCell="E7" sqref="E7"/>
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+      <selection activeCell="B10" sqref="B10"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
       <selection activeCell="C8" sqref="C8"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="B10" sqref="B10"/>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" showPageBreaks="1">
+      <selection activeCell="E7" sqref="E7"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1777,9 +1934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1789,9 +1944,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>73</v>
-      </c>
+      <c r="A1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1875,7 +2034,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -1892,7 +2051,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -1931,10 +2090,10 @@
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>50</v>
@@ -1943,15 +2102,15 @@
         <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>56</v>
@@ -1960,12 +2119,12 @@
         <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>55</v>
@@ -1977,15 +2136,15 @@
         <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>56</v>
@@ -1994,15 +2153,15 @@
         <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>56</v>
@@ -2011,15 +2170,15 @@
         <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>56</v>
@@ -2028,27 +2187,26 @@
         <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" topLeftCell="A10">
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
     <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" topLeftCell="A10">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2062,7 +2220,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2075,7 +2233,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2143,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -2165,7 +2323,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}">
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
       <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2175,7 +2333,7 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}">
       <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2192,9 +2350,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2344,26 +2505,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2387,9 +2537,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added T14 - Shared Trip Authorized.
</commit_message>
<xml_diff>
--- a/TNP Reporting Manual.xlsx
+++ b/TNP Reporting Manual.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="107">
   <si>
     <t>Element</t>
   </si>
@@ -496,6 +496,15 @@
       </rPr>
       <t xml:space="preserve"> during the reporting period.  Trips in progress at the end of the reporting period should be held for the next report.  For the purposes of this file, a trip is a transaction with a specific customer, including any additional people transported under the same transaction. A transaction with a different customer, even if present in the vehicle at the same time, is a separate trip.</t>
     </r>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shared Trip Authorized </t>
+  </si>
+  <si>
+    <t>Did the customer agree to a shared trip, regardless of whether the trip was actually shared. Enter Y or N only.</t>
   </si>
 </sst>
 </file>
@@ -699,7 +708,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{71B4191B-0BAA-4279-8855-B887A7C7CB4D}" diskRevisions="1" revisionId="90" version="12">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A0A17979-3394-45AD-849D-A36C2EA098FB}" diskRevisions="1" revisionId="96" version="13">
   <header guid="{88FB6579-DFE5-4318-B552-D049D04FAB73}" dateTime="2016-10-13T12:50:22" maxSheetId="5" userName="Jonathan Levy" r:id="rId16" minRId="76">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -784,6 +793,15 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{A0A17979-3394-45AD-849D-A36C2EA098FB}" dateTime="2017-05-15T15:47:21" maxSheetId="6" userName="Jonathan Levy" r:id="rId26" minRId="91" maxRId="96">
+    <sheetIdMap count="5">
+      <sheetId val="5"/>
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -947,6 +965,72 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="91" sId="3" eol="1" ref="A16:XFD16" action="insertRow"/>
+  <rcc rId="92" sId="3">
+    <nc r="A16" t="inlineStr">
+      <is>
+        <t>T14</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="A16">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="93" sId="3">
+    <nc r="B16" t="inlineStr">
+      <is>
+        <t xml:space="preserve">Shared Trip Authorized </t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="B16">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="94" sId="3">
+    <nc r="C16" t="inlineStr">
+      <is>
+        <t>String</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="C16">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="95" sId="3">
+    <nc r="D16" t="inlineStr">
+      <is>
+        <t>Yes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="D16">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="96" sId="3">
+    <nc r="E16" t="inlineStr">
+      <is>
+        <t>Did the customer agree to a shared trip, regardless of whether the trip was actually shared. Enter Y or N only.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="E16">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
@@ -1202,7 +1286,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{71B4191B-0BAA-4279-8855-B887A7C7CB4D}" name="Jonathan Levy" id="-1743086255" dateTime="2017-05-15T14:18:15"/>
+  <userInfo guid="{A0A17979-3394-45AD-849D-A36C2EA098FB}" name="Jonathan Levy" id="-1743086255" dateTime="2017-05-15T14:18:15"/>
 </users>
 </file>
 
@@ -1932,9 +2016,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2188,6 +2274,23 @@
       </c>
       <c r="E15" s="3" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added V10 (WAV) and V11 (Vehicle Inspection Date).
</commit_message>
<xml_diff>
--- a/TNP Reporting Manual.xlsx
+++ b/TNP Reporting Manual.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="22620" windowHeight="13170" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="22620" windowHeight="13170" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="File Names" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
   <si>
     <t>Element</t>
   </si>
@@ -505,6 +505,24 @@
   </si>
   <si>
     <t>Did the customer agree to a shared trip, regardless of whether the trip was actually shared. Enter Y or N only.</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>WAV</t>
+  </si>
+  <si>
+    <t>Was this vehicle approved by the City of Chicago as a Wheelchair Accessible Vehicle, with that approval being valid on the last day of the reporting period? Enter Y or N only.</t>
+  </si>
+  <si>
+    <t>V11</t>
+  </si>
+  <si>
+    <t>Vehicle Inspection Date</t>
+  </si>
+  <si>
+    <t>The date (no time) when the vehicle was last inspected by a City of Chicago authorized facility and found to be in compliance with all requirements necessary for operating the vehicle for TNP services.</t>
   </si>
 </sst>
 </file>
@@ -708,7 +726,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A0A17979-3394-45AD-849D-A36C2EA098FB}" diskRevisions="1" revisionId="96" version="13">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{674B264A-9C3B-4E20-9E96-D8FB54253BC5}" diskRevisions="1" revisionId="108" version="14">
   <header guid="{88FB6579-DFE5-4318-B552-D049D04FAB73}" dateTime="2016-10-13T12:50:22" maxSheetId="5" userName="Jonathan Levy" r:id="rId16" minRId="76">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -802,6 +820,15 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{674B264A-9C3B-4E20-9E96-D8FB54253BC5}" dateTime="2017-05-15T15:53:13" maxSheetId="6" userName="Jonathan Levy" r:id="rId27" minRId="97" maxRId="108">
+    <sheetIdMap count="5">
+      <sheetId val="5"/>
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1031,6 +1058,128 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="97" sId="2" eol="1" ref="A12:XFD12" action="insertRow"/>
+  <rcc rId="98" sId="2">
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>V10</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="A12">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="99" sId="2">
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>WAV</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="B12">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="100" sId="2">
+    <nc r="C12" t="inlineStr">
+      <is>
+        <t>String</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="C12">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="101" sId="2">
+    <nc r="D12" t="inlineStr">
+      <is>
+        <t>Yes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="D12">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="102" sId="2">
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Was this vehicle approved by the City of Chicago as a Wheelchair Accessible Vehicle, with that approval being valid on the last day of the reporting period? Enter Y or N only.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="E12">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rrc rId="103" sId="2" eol="1" ref="A13:XFD13" action="insertRow"/>
+  <rcc rId="104" sId="2">
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>V11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="A13">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="105" sId="2">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>Vehicle Inspection Date</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="B13">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="106" sId="2" xfDxf="1" dxf="1">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>ISO 8601</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="107" sId="2">
+    <nc r="D13" t="inlineStr">
+      <is>
+        <t>Yes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="D13">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="108" sId="2">
+    <nc r="E13" t="inlineStr">
+      <is>
+        <t>The date (no time) when the vehicle was last inspected by a City of Chicago authorized facility and found to be in compliance with all requirements necessary for operating the vehicle for TNP services.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="E13">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
@@ -1284,9 +1433,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{A0A17979-3394-45AD-849D-A36C2EA098FB}" name="Jonathan Levy" id="-1743086255" dateTime="2017-05-15T14:18:15"/>
+  <userInfo guid="{674B264A-9C3B-4E20-9E96-D8FB54253BC5}" name="Jonathan Levy" id="-1743086255" dateTime="2017-05-15T14:18:15"/>
 </users>
 </file>
 
@@ -1614,9 +1763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1798,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1984,6 +2131,40 @@
       </c>
       <c r="E11" s="3" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2018,8 +2199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added T15 (Shared Trip ID).
</commit_message>
<xml_diff>
--- a/TNP Reporting Manual.xlsx
+++ b/TNP Reporting Manual.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,8 +21,8 @@
   <calcPr calcId="140000"/>
   <customWorkbookViews>
     <customWorkbookView name="Jonathan Levy - Personal View" guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1066" tabRatio="500" activeSheetId="3"/>
+    <customWorkbookView name="MONIQUE - Personal View" guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="785" tabRatio="500" activeSheetId="2"/>
     <customWorkbookView name="Unisys - Personal View" guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="MONIQUE - Personal View" guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="785" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="116">
   <si>
     <t>Element</t>
   </si>
@@ -523,6 +523,15 @@
   </si>
   <si>
     <t>The date (no time) when the vehicle was last inspected by a City of Chicago authorized facility and found to be in compliance with all requirements necessary for operating the vehicle for TNP services.</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>Shared Trip ID</t>
+  </si>
+  <si>
+    <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
   </si>
 </sst>
 </file>
@@ -642,7 +651,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -664,6 +673,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -726,56 +738,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{674B264A-9C3B-4E20-9E96-D8FB54253BC5}" diskRevisions="1" revisionId="108" version="14">
-  <header guid="{88FB6579-DFE5-4318-B552-D049D04FAB73}" dateTime="2016-10-13T12:50:22" maxSheetId="5" userName="Jonathan Levy" r:id="rId16" minRId="76">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D49C6F83-5611-404A-B6D0-68B98F314D93}" dateTime="2016-10-13T12:50:46" maxSheetId="5" userName="Jonathan Levy" r:id="rId17">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{903E2346-E1C1-427A-B14C-DE5BD6FA8D95}" dateTime="2016-10-13T12:52:26" maxSheetId="5" userName="Jonathan Levy" r:id="rId18" minRId="77" maxRId="78">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{04AE151E-461F-488D-BB49-12FBA8EBDD7A}" dateTime="2016-10-13T13:40:53" maxSheetId="5" userName="Jonathan Levy" r:id="rId19" minRId="79" maxRId="82">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{9397DBB6-AE3B-424D-BA11-0283E19A5355}" dateTime="2016-10-13T13:44:55" maxSheetId="5" userName="Jonathan Levy" r:id="rId20">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1DEDC259-0305-4062-86FB-2A93864D10D4}" dateTime="2016-10-13T13:47:17" maxSheetId="5" userName="Jonathan Levy" r:id="rId21" minRId="83" maxRId="84">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{FDBC06D3-9E0D-4DCA-9B0A-EAB13DF0C855}" dateTime="2016-10-13T15:27:25" maxSheetId="6" userName="Jonathan Levy" r:id="rId22" minRId="85" maxRId="87">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{292834E9-302B-4C7E-A04E-BCA93BF8E0C7}" diskRevisions="1" revisionId="116" version="18">
+  <header guid="{91928FF6-78F8-4D0D-AED5-CBCADDF7415D}" dateTime="2017-07-28T16:35:53" maxSheetId="6" userName="Jonathan Levy" r:id="rId28" minRId="109" maxRId="114">
     <sheetIdMap count="5">
       <sheetId val="5"/>
       <sheetId val="1"/>
@@ -784,7 +748,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{9DFAB7F4-9EC9-4A0F-ACF7-77494652790A}" dateTime="2016-10-14T11:37:08" maxSheetId="6" userName="Jonathan Levy" r:id="rId23" minRId="88">
+  <header guid="{624635B8-F213-48E7-AF2E-7302F6A130BF}" dateTime="2017-07-28T16:37:23" maxSheetId="6" userName="Jonathan Levy" r:id="rId29" minRId="115">
     <sheetIdMap count="5">
       <sheetId val="5"/>
       <sheetId val="1"/>
@@ -793,7 +757,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{DA3DC931-C2F3-483F-A5F5-1B1BEE67700A}" dateTime="2016-10-14T11:37:36" maxSheetId="6" userName="Jonathan Levy" r:id="rId24" minRId="89">
+  <header guid="{D3C7FCDB-E057-44FD-BD06-B679E9D68780}" dateTime="2017-07-28T16:41:12" maxSheetId="6" userName="Jonathan Levy" r:id="rId30">
     <sheetIdMap count="5">
       <sheetId val="5"/>
       <sheetId val="1"/>
@@ -802,25 +766,7 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{71B4191B-0BAA-4279-8855-B887A7C7CB4D}" dateTime="2017-05-15T15:44:47" maxSheetId="6" userName="Jonathan Levy" r:id="rId25" minRId="90">
-    <sheetIdMap count="5">
-      <sheetId val="5"/>
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{A0A17979-3394-45AD-849D-A36C2EA098FB}" dateTime="2017-05-15T15:47:21" maxSheetId="6" userName="Jonathan Levy" r:id="rId26" minRId="91" maxRId="96">
-    <sheetIdMap count="5">
-      <sheetId val="5"/>
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{674B264A-9C3B-4E20-9E96-D8FB54253BC5}" dateTime="2017-05-15T15:53:13" maxSheetId="6" userName="Jonathan Levy" r:id="rId27" minRId="97" maxRId="108">
+  <header guid="{292834E9-302B-4C7E-A04E-BCA93BF8E0C7}" dateTime="2017-07-28T16:44:07" maxSheetId="6" userName="Jonathan Levy" r:id="rId31" minRId="116">
     <sheetIdMap count="5">
       <sheetId val="5"/>
       <sheetId val="1"/>
@@ -834,609 +780,118 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="76" sId="1">
-    <oc r="E5" t="inlineStr">
+  <rrc rId="109" sId="3" eol="1" ref="A17:XFD17" action="insertRow"/>
+  <rcc rId="110" sId="3">
+    <nc r="A17" t="inlineStr">
       <is>
-        <t>The state illussing the driver's license that is listed on the driver's license number.</t>
+        <t>T15</t>
       </is>
-    </oc>
-    <nc r="E5" t="inlineStr">
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="A17">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="B17">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="111" sId="3">
+    <nc r="C17" t="inlineStr">
       <is>
-        <t>The state issuing the driver's license that is listed on the driver's license number</t>
+        <t>String</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="C17">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="112" sId="3">
+    <nc r="D17" t="inlineStr">
+      <is>
+        <t>Yes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="D17">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="3" sqref="E17">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="113" sId="3">
+    <nc r="B17" t="inlineStr">
+      <is>
+        <t>Shared Trip ID</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="114" sId="3">
+    <nc r="E17" t="inlineStr">
+      <is>
+        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered intothis field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
       </is>
     </nc>
   </rcc>
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="3" sqref="A1" start="0" length="0">
-    <dxf>
-      <alignment vertical="top" wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1">
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1">
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1" start="0" length="0">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1">
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1" start="0" length="0">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1">
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1" start="0" length="0">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="A1:E1">
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="90" sId="3">
-    <oc r="A1" t="inlineStr">
+  <rcc rId="115" sId="3">
+    <oc r="E17" t="inlineStr">
       <is>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Scope: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">All Trips </t>
-        </r>
-        <r>
-          <rPr>
-            <u/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>completed</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> during the reporting period.  Trips in progress at the end of the reporting period should be held for the next report.</t>
-        </r>
+        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered intothis field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
       </is>
     </oc>
-    <nc r="A1" t="inlineStr">
+    <nc r="E17" t="inlineStr">
       <is>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Scope: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">All Trips </t>
-        </r>
-        <r>
-          <rPr>
-            <u/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>completed</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> during the reporting period.  Trips in progress at the end of the reporting period should be held for the next report.  For the purposes of this file, a trip is a transaction with a specific customer, including any additional people transported under the same transaction. A transaction with a different customer, even if present in the vehicle at the same time, is a separate trip.</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="91" sId="3" eol="1" ref="A16:XFD16" action="insertRow"/>
-  <rcc rId="92" sId="3">
-    <nc r="A16" t="inlineStr">
-      <is>
-        <t>T14</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="A16">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="93" sId="3">
-    <nc r="B16" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Shared Trip Authorized </t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="B16">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="94" sId="3">
-    <nc r="C16" t="inlineStr">
-      <is>
-        <t>String</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="C16">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="95" sId="3">
-    <nc r="D16" t="inlineStr">
-      <is>
-        <t>Yes</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="D16">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="96" sId="3">
-    <nc r="E16" t="inlineStr">
-      <is>
-        <t>Did the customer agree to a shared trip, regardless of whether the trip was actually shared. Enter Y or N only.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="E16">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="97" sId="2" eol="1" ref="A12:XFD12" action="insertRow"/>
-  <rcc rId="98" sId="2">
-    <nc r="A12" t="inlineStr">
-      <is>
-        <t>V10</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A12">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="99" sId="2">
-    <nc r="B12" t="inlineStr">
-      <is>
-        <t>WAV</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B12">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="100" sId="2">
-    <nc r="C12" t="inlineStr">
-      <is>
-        <t>String</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="C12">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="101" sId="2">
-    <nc r="D12" t="inlineStr">
-      <is>
-        <t>Yes</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="D12">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="102" sId="2">
-    <nc r="E12" t="inlineStr">
-      <is>
-        <t>Was this vehicle approved by the City of Chicago as a Wheelchair Accessible Vehicle, with that approval being valid on the last day of the reporting period? Enter Y or N only.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="E12">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rrc rId="103" sId="2" eol="1" ref="A13:XFD13" action="insertRow"/>
-  <rcc rId="104" sId="2">
-    <nc r="A13" t="inlineStr">
-      <is>
-        <t>V11</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A13">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="105" sId="2">
-    <nc r="B13" t="inlineStr">
-      <is>
-        <t>Vehicle Inspection Date</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B13">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="106" sId="2" xfDxf="1" dxf="1">
-    <nc r="C13" t="inlineStr">
-      <is>
-        <t>ISO 8601</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="107" sId="2">
-    <nc r="D13" t="inlineStr">
-      <is>
-        <t>Yes</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="D13">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="108" sId="2">
-    <nc r="E13" t="inlineStr">
-      <is>
-        <t>The date (no time) when the vehicle was last inspected by a City of Chicago authorized facility and found to be in compliance with all requirements necessary for operating the vehicle for TNP services.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="E13">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" xfDxf="1" sqref="E5" start="0" length="0">
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="77" sId="2">
-    <oc r="E5" t="inlineStr">
-      <is>
-        <t>The issuing state of the license plate in this file</t>
-      </is>
-    </oc>
-    <nc r="E5" t="inlineStr">
-      <is>
-        <t>The state issuing the license plate</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="78" sId="1">
-    <oc r="E5" t="inlineStr">
-      <is>
-        <t>The state issuing the driver's license that is listed on the driver's license number</t>
-      </is>
-    </oc>
-    <nc r="E5" t="inlineStr">
-      <is>
-        <t>The state issuing the driver's license</t>
+        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
       </is>
     </nc>
   </rcc>
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="2" sqref="C1:C1048576">
+    <dxf>
+      <alignment vertical="top"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
+  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="79" sId="2">
-    <oc r="E8" t="inlineStr">
+  <rcc rId="116" sId="3">
+    <oc r="E17" t="inlineStr">
       <is>
-        <t>A description of the vehicle's color, defined by the manufacturer, the car owner, or the driver.</t>
+        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
       </is>
     </oc>
-    <nc r="E8" t="inlineStr">
+    <nc r="E17" t="inlineStr">
       <is>
-        <t>A description of the vehicle's color, defined by the manufacturer, the car owner, or the driver</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="80" sId="2">
-    <oc r="E9" t="inlineStr">
-      <is>
-        <t>The model year of the vehicle advertised by the manufacturer.</t>
-      </is>
-    </oc>
-    <nc r="E9" t="inlineStr">
-      <is>
-        <t>The model year of the vehicle, as advertised by the manufacturer</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="81" sId="2">
-    <oc r="E10" t="inlineStr">
-      <is>
-        <t>The driver's license number(s) of the driver(s) authorized to operate this vehicle for your company's service. If multiple drivers are authorized to drive the vehicle, then use a pipe character ("|", ASCII 166) to deliminate each driver. Any driver's license number listed in this field should be included in the DRIVER file submitted in field D2.</t>
-      </is>
-    </oc>
-    <nc r="E10" t="inlineStr">
-      <is>
-        <t>The driver's license number(s) of the driver(s) authorized to operate this vehicle for your company's service. If multiple drivers are authorized to drive the vehicle, then submit multiple vehicle records, one for each driver with all fields except V8 and V9 being the same. Any driver's license number listed in this field should be included in the DRIVER file submitted in field D2.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="82" sId="2">
-    <oc r="E11" t="inlineStr">
-      <is>
-        <t>The driver's license state(s) of the driver(s) authorized to operate this vehicle for your company's service. If multiple drivers are authorized to drive the vehicle, then use a pipe character ("|", ASCII 166) to deliminate each driver and should be listed respectively with the entries in V8. The state listed in this file should correspond to the state listed in D3.</t>
-      </is>
-    </oc>
-    <nc r="E11" t="inlineStr">
-      <is>
-        <t>The driver's license state(s) of the driver(s) authorized to operate this vehicle for your company's service. If multiple drivers are authorized to drive the vehicle,then submit multiple vehicle records, one for each driver with all fields except V8 and V9 being the same. The state listed in this file should correspond to the state listed in D3.</t>
+        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
       </is>
     </nc>
   </rcc>
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcmt sheetId="3" cell="E6" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Jonathan Levy"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="83" sId="3">
-    <oc r="E14" t="inlineStr">
-      <is>
-        <t>The total taxes and fees charged to the consumer, including any "pick-up" or other taxes. The amount 0.00 should be used if no taxes or fees were charged.</t>
-      </is>
-    </oc>
-    <nc r="E14" t="inlineStr">
-      <is>
-        <t>The total taxes and fees charged to the consumer, including any "pick-up" or other taxes. The amount 0.00 should be used if no taxes or fees were charged. Do not use currency symbols.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="84" sId="3">
-    <oc r="E11" t="inlineStr">
-      <is>
-        <t>The total cost, including tip, taxes, and all charges, charged to the customer. This elements should equal the sum of T8, T9, T10, and T11.</t>
-      </is>
-    </oc>
-    <nc r="E11" t="inlineStr">
-      <is>
-        <t>The total cost, including tip, taxes, and all charges, charged to the customer. Do not use currency symbols. This elements should equal the sum of T10, T11, T12, and T13.</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <ris rId="85" sheetId="5" name="[TNP Reporting Manual.xlsx]File Names" sheetPosition="1"/>
-  <rfmt sheetId="5" xfDxf="1" sqref="A1" start="0" length="0"/>
-  <rfmt sheetId="5" xfDxf="1" sqref="A2" start="0" length="0"/>
-  <rfmt sheetId="5" sqref="A1:A1048576">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="86" sId="5">
-    <nc r="A2" t="inlineStr">
-      <is>
-        <t>[company]-[topic]-[date].csv</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="87" sId="5">
-    <nc r="A1" t="inlineStr">
-      <is>
-        <r>
-          <t xml:space="preserve">Submit four separate CSV files with the following naming convention, where [company] denotes the submitting company, [topic] represents one of the four areas being requested: driver, vehicle, trip, and session, and date corresponds to the period </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>covered</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> by the file (not the period when the file is submitted). For instance, ACME service submitting the driver file of drivers eligible in March 2016 would submit acme-driver-201603.csv.</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcmt sheetId="3" cell="E7" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Jonathan Levy"/>
-  <rcc rId="88" sId="3">
-    <oc r="E7" t="inlineStr">
-      <is>
-        <t>The Census Block 2010 corresponding to the starting location of the trip.</t>
-      </is>
-    </oc>
-    <nc r="E7" t="inlineStr">
-      <is>
-        <r>
-          <t xml:space="preserve">The Census Block 2010 corresponding to the starting location of the trip.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.  TNPs interested in doing so should discuss it with the City of Chicago.)</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="89" sId="3">
-    <oc r="E7" t="inlineStr">
-      <is>
-        <r>
-          <t xml:space="preserve">The Census Block 2010 corresponding to the starting location of the trip.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.  TNPs interested in doing so should discuss it with the City of Chicago.)</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="E7" t="inlineStr">
-      <is>
-        <r>
-          <t xml:space="preserve">The Census Block 2010 corresponding to the starting location of the trip.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note: Reporting Latitude and Longitude for this field and T7 instead of Census Blocks is acceptable by special arrangement.)</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{674B264A-9C3B-4E20-9E96-D8FB54253BC5}" name="Jonathan Levy" id="-1743086255" dateTime="2017-05-15T14:18:15"/>
-</users>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1783,7 +1238,6 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -1797,9 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1918,19 +1370,18 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" scale="125" showPageBreaks="1">
+      <selection activeCell="D11" sqref="D11"/>
+      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
     <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" scale="125">
       <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-    </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" scale="125" showPageBreaks="1">
-      <selection activeCell="D11" sqref="D11"/>
-      <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1947,14 +1398,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1970,7 +1419,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2157,7 +1606,7 @@
       <c r="B13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -2170,23 +1619,22 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
-      <selection activeCell="B10" sqref="B10"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" showPageBreaks="1">
+      <selection activeCell="E7" sqref="E7"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
       <selection activeCell="C8" sqref="C8"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" showPageBreaks="1">
-      <selection activeCell="E7" sqref="E7"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2197,17 +1645,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.875" customWidth="1"/>
+    <col min="5" max="5" width="71.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2253,7 +1699,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -2304,7 +1750,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
@@ -2321,7 +1767,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -2338,7 +1784,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -2406,7 +1852,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>84</v>
       </c>
@@ -2440,7 +1886,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>91</v>
       </c>
@@ -2472,6 +1918,23 @@
       </c>
       <c r="E16" s="3" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2480,11 +1943,11 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" topLeftCell="A10">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" topLeftCell="A10">
+    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -2503,9 +1966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2608,17 +2069,16 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}">
       <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
       <selection activeCell="F7" sqref="F7"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}">
-      <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -2634,12 +2094,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2789,15 +2246,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2821,17 +2289,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Clarified the T15 description.
</commit_message>
<xml_diff>
--- a/TNP Reporting Manual.xlsx
+++ b/TNP Reporting Manual.xlsx
@@ -20,9 +20,9 @@
   </sheets>
   <calcPr calcId="140000"/>
   <customWorkbookViews>
+    <customWorkbookView name="Unisys - Personal View" guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="MONIQUE - Personal View" guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="785" tabRatio="500" activeSheetId="2"/>
     <customWorkbookView name="Jonathan Levy - Personal View" guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1066" tabRatio="500" activeSheetId="3"/>
-    <customWorkbookView name="MONIQUE - Personal View" guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="785" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Unisys - Personal View" guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -531,7 +531,7 @@
     <t>Shared Trip ID</t>
   </si>
   <si>
-    <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
+    <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs. Therefore the IDs need only be unique within a TNP, not between TNPs.  However, within that TNP, the ID must be permanently unique, not just unique within the reporting period. Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{292834E9-302B-4C7E-A04E-BCA93BF8E0C7}" diskRevisions="1" revisionId="116" version="18">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A2F260D8-ADF4-43F9-A9FC-4E98D6AD2A55}" diskRevisions="1" revisionId="117" version="19">
   <header guid="{91928FF6-78F8-4D0D-AED5-CBCADDF7415D}" dateTime="2017-07-28T16:35:53" maxSheetId="6" userName="Jonathan Levy" r:id="rId28" minRId="109" maxRId="114">
     <sheetIdMap count="5">
       <sheetId val="5"/>
@@ -767,6 +767,15 @@
     </sheetIdMap>
   </header>
   <header guid="{292834E9-302B-4C7E-A04E-BCA93BF8E0C7}" dateTime="2017-07-28T16:44:07" maxSheetId="6" userName="Jonathan Levy" r:id="rId31" minRId="116">
+    <sheetIdMap count="5">
+      <sheetId val="5"/>
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A2F260D8-ADF4-43F9-A9FC-4E98D6AD2A55}" dateTime="2017-08-09T11:46:33" maxSheetId="6" userName="Jonathan Levy" r:id="rId32" minRId="117">
     <sheetIdMap count="5">
       <sheetId val="5"/>
       <sheetId val="1"/>
@@ -884,6 +893,23 @@
     <nc r="E17" t="inlineStr">
       <is>
         <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="117" sId="3">
+    <oc r="E17" t="inlineStr">
+      <is>
+        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
+      </is>
+    </oc>
+    <nc r="E17" t="inlineStr">
+      <is>
+        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs. Therefore the IDs need only be unique within a TNP, not between TNPs.  However, within that TNP, the ID must be permanently unique, not just unique within the reporting period. Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
       </is>
     </nc>
   </rcc>
@@ -1369,19 +1395,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" scale="125">
+      <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
     <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" scale="125" showPageBreaks="1">
       <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}" scale="125">
-      <selection activeCell="A2" sqref="A2"/>
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1618,19 +1644,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
+      <selection activeCell="C8" sqref="C8"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" showPageBreaks="1">
       <selection activeCell="E7" sqref="E7"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+      <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
-      <selection activeCell="C8" sqref="C8"/>
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1647,7 +1673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1939,17 +1967,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{E7F956AB-6F75-4CEC-B118-18C87133E3F9}" topLeftCell="A10">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2068,7 +2096,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
+    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
+      <selection activeCell="F7" sqref="F7"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -2077,8 +2106,7 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{ECE95F91-A1E0-4226-9A93-B89D81B31E4B}">
-      <selection activeCell="F7" sqref="F7"/>
+    <customSheetView guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -2094,9 +2122,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2246,26 +2277,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2289,9 +2309,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63CD73AF-6623-49CE-90C6-8A2D589829ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{897524F9-A65A-4925-ABCD-0B3F9EC61E0A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1dab034a-a369-4676-a76a-0f9f39450218"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lots of changes, just getting it to work
</commit_message>
<xml_diff>
--- a/TNP Reporting Manual.xlsx
+++ b/TNP Reporting Manual.xlsx
@@ -739,42 +739,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A2F260D8-ADF4-43F9-A9FC-4E98D6AD2A55}" diskRevisions="1" revisionId="117" version="19">
-  <header guid="{91928FF6-78F8-4D0D-AED5-CBCADDF7415D}" dateTime="2017-07-28T16:35:53" maxSheetId="6" userName="Jonathan Levy" r:id="rId28" minRId="109" maxRId="114">
-    <sheetIdMap count="5">
-      <sheetId val="5"/>
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{624635B8-F213-48E7-AF2E-7302F6A130BF}" dateTime="2017-07-28T16:37:23" maxSheetId="6" userName="Jonathan Levy" r:id="rId29" minRId="115">
-    <sheetIdMap count="5">
-      <sheetId val="5"/>
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D3C7FCDB-E057-44FD-BD06-B679E9D68780}" dateTime="2017-07-28T16:41:12" maxSheetId="6" userName="Jonathan Levy" r:id="rId30">
-    <sheetIdMap count="5">
-      <sheetId val="5"/>
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{292834E9-302B-4C7E-A04E-BCA93BF8E0C7}" dateTime="2017-07-28T16:44:07" maxSheetId="6" userName="Jonathan Levy" r:id="rId31" minRId="116">
-    <sheetIdMap count="5">
-      <sheetId val="5"/>
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
   <header guid="{A2F260D8-ADF4-43F9-A9FC-4E98D6AD2A55}" dateTime="2017-08-09T11:46:33" maxSheetId="6" userName="Jonathan Levy" r:id="rId32" minRId="117">
     <sheetIdMap count="5">
       <sheetId val="5"/>
@@ -785,118 +749,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="109" sId="3" eol="1" ref="A17:XFD17" action="insertRow"/>
-  <rcc rId="110" sId="3">
-    <nc r="A17" t="inlineStr">
-      <is>
-        <t>T15</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="A17">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="B17">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="111" sId="3">
-    <nc r="C17" t="inlineStr">
-      <is>
-        <t>String</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="C17">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="112" sId="3">
-    <nc r="D17" t="inlineStr">
-      <is>
-        <t>Yes</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="D17">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="3" sqref="E17">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="113" sId="3">
-    <nc r="B17" t="inlineStr">
-      <is>
-        <t>Shared Trip ID</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="114" sId="3">
-    <nc r="E17" t="inlineStr">
-      <is>
-        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered intothis field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="115" sId="3">
-    <oc r="E17" t="inlineStr">
-      <is>
-        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered intothis field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
-      </is>
-    </oc>
-    <nc r="E17" t="inlineStr">
-      <is>
-        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="C1:C1048576">
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-  </rfmt>
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="delete"/>
-  <rcv guid="{D4D96072-2E99-4CEB-98D6-D44DA43E9BBA}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="116" sId="3">
-    <oc r="E17" t="inlineStr">
-      <is>
-        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
-      </is>
-    </oc>
-    <nc r="E17" t="inlineStr">
-      <is>
-        <t>Each complete empty-to-empty run of a vehicle should be assigned a unique ID and this ID should be entered into this field. The ID should be a non-case-sensitive string value with any letters represented in their capital forms. Each TNP may use a coding system of its liking to assign the IDs, although the City of Chicago reserves the right to apply further restrictions, as it finds necessary. Therefore the IDs need only be unique within a TNP, not between TNPs.  Every trip record within the empty-to-empty run should list the same Shared Trip ID.</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>